<commit_message>
Bug fixes when adding a point
</commit_message>
<xml_diff>
--- a/src/backend/Records/prueba final rpb_RPB.xlsx
+++ b/src/backend/Records/prueba final rpb_RPB.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,14 +463,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t xml:space="preserve">BEAMU-RH </t>
+          <t xml:space="preserve">BEAML-RH </t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>4953</v>
+        <v>6475</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -486,41 +486,41 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DOORFRAME</t>
+          <t xml:space="preserve">BEAMU-RH </t>
         </is>
       </c>
       <c r="B3" t="n">
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1337</v>
+        <v>4961</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3A</t>
+          <t>Delaminacion</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Lower</t>
+          <t>Right</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t xml:space="preserve">BEAML-RH </t>
+          <t xml:space="preserve">BEAMU-RH </t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>5938</v>
+        <v>4953</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>NC</t>
+          <t>-</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -532,67 +532,113 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BMCJ-RE-RH-LW</t>
+          <t>DOORFRAME</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" t="n">
-        <v>6579</v>
+        <v>1337</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>3A</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Right</t>
+          <t>Lower</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t xml:space="preserve">BMCJ-LH </t>
+          <t xml:space="preserve">BEAML-RH </t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>6547</v>
+        <v>5938</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2da Sobremedida</t>
+          <t>NC</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Left</t>
+          <t>Right</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>BMCJ-RE-RH-LW</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>6579</v>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Right</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BMCJ-LH </t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="n">
+        <v>6547</v>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>2da Sobremedida</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Left</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
           <t xml:space="preserve">BEAMU-LH </t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="B9" t="n">
         <v>1</v>
       </c>
-      <c r="C7" t="n">
+      <c r="C9" t="n">
         <v>4568</v>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>1ra Sobremedida</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>Left</t>
         </is>

</xml_diff>